<commit_message>
Final polish with full revised M4.
</commit_message>
<xml_diff>
--- a/data_input/maiz_soil_params_irr.xlsx
+++ b/data_input/maiz_soil_params_irr.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pyaez_github_test_env\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pyaez_github_test_env\input\new soil evaluation\KB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2FA6D4-66CC-4A7C-83A3-4077BC02A089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B7CC34-7012-433A-AB4B-10D8601E3D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="2" xr2:uid="{8AAD9566-BB4C-44D2-B3CE-FD7B121B3AA5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="4" xr2:uid="{8AAD9566-BB4C-44D2-B3CE-FD7B121B3AA5}"/>
   </bookViews>
   <sheets>
     <sheet name="SQ1" sheetId="1" r:id="rId1"/>
@@ -42,16 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="49">
-  <si>
-    <t>Fine</t>
-  </si>
-  <si>
-    <t>Medium</t>
-  </si>
-  <si>
-    <t>Coarse</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="51">
   <si>
     <t>TXT_fct</t>
   </si>
@@ -104,12 +95,6 @@
     <t>Lithic</t>
   </si>
   <si>
-    <t>skeletic</t>
-  </si>
-  <si>
-    <t>hyperskeletic</t>
-  </si>
-  <si>
     <t>OSD_val</t>
   </si>
   <si>
@@ -189,6 +174,27 @@
   </si>
   <si>
     <t>CECclay_fct</t>
+  </si>
+  <si>
+    <t>Clay (light)</t>
+  </si>
+  <si>
+    <t>Clay loam</t>
+  </si>
+  <si>
+    <t>Sandy clay</t>
+  </si>
+  <si>
+    <t>Loam</t>
+  </si>
+  <si>
+    <t>Sandy clay loam</t>
+  </si>
+  <si>
+    <t>Skeletic</t>
+  </si>
+  <si>
+    <t>Hyperskeletic</t>
   </si>
 </sst>
 </file>
@@ -542,81 +548,94 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FACB6447-EEBE-4CDF-97EB-75A776AA2E7F}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="C2">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="D2">
-        <v>30</v>
+        <v>100</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="F2">
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="C3">
         <v>0.8</v>
       </c>
       <c r="D3">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C4">
+        <v>90</v>
+      </c>
+      <c r="D4">
         <v>70</v>
       </c>
-      <c r="D4">
-        <v>90</v>
-      </c>
       <c r="E4">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>3.6</v>
@@ -639,7 +658,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -662,42 +681,42 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>3.5</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
         <v>0</v>
-      </c>
-      <c r="C7">
-        <v>1.6</v>
-      </c>
-      <c r="D7">
-        <v>2.8</v>
-      </c>
-      <c r="E7">
-        <v>4</v>
-      </c>
-      <c r="F7">
-        <v>6.5</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B8">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="C8">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="D8">
         <v>70</v>
       </c>
       <c r="E8">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="F8">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -709,7 +728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C1CF382-BD27-4D55-8B33-6E3E46737D1E}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -720,178 +739,172 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="C2">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="D2">
-        <v>30</v>
+        <v>100</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="F2">
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="C3">
         <v>35</v>
       </c>
       <c r="D3">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="E3">
-        <v>80</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C4">
+        <v>90</v>
+      </c>
+      <c r="D4">
         <v>70</v>
       </c>
-      <c r="D4">
-        <v>90</v>
-      </c>
       <c r="E4">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
         <v>2</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <v>8</v>
-      </c>
-      <c r="F5">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B6">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="C6">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="D6">
         <v>70</v>
       </c>
-      <c r="E6">
-        <v>90</v>
-      </c>
-      <c r="F6">
-        <v>100</v>
-      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B7">
+        <v>16</v>
+      </c>
+      <c r="C7">
         <v>0</v>
-      </c>
-      <c r="C7">
-        <v>16</v>
-      </c>
-      <c r="D7">
-        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B8">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="C8">
         <v>90</v>
       </c>
-      <c r="D8">
-        <v>100</v>
-      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B9">
-        <v>3.6</v>
+        <v>5.8</v>
       </c>
       <c r="C9">
-        <v>4.0999999999999996</v>
+        <v>5.5</v>
       </c>
       <c r="D9">
-        <v>4.5</v>
+        <v>5.2</v>
       </c>
       <c r="E9">
-        <v>5</v>
+        <v>4.7</v>
       </c>
       <c r="F9">
-        <v>5.5</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="G9">
-        <v>6</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B10">
+        <v>100</v>
+      </c>
+      <c r="C10">
+        <v>90</v>
+      </c>
+      <c r="D10">
+        <v>70</v>
+      </c>
+      <c r="E10">
+        <v>50</v>
+      </c>
+      <c r="F10">
+        <v>30</v>
+      </c>
+      <c r="G10">
         <v>10</v>
-      </c>
-      <c r="C10">
-        <v>30</v>
-      </c>
-      <c r="D10">
-        <v>50</v>
-      </c>
-      <c r="E10">
-        <v>70</v>
-      </c>
-      <c r="F10">
-        <v>90</v>
-      </c>
-      <c r="G10">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -901,10 +914,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DC60B64-85DA-4C3E-886C-1B30B1A1B4F3}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -912,51 +925,69 @@
     <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B1">
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="C1">
+        <v>85</v>
+      </c>
+      <c r="D1">
         <v>70</v>
       </c>
-      <c r="D1">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1">
+        <v>30</v>
+      </c>
+      <c r="F1">
+        <v>20</v>
+      </c>
+      <c r="G1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B2">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C2">
         <v>90</v>
       </c>
       <c r="D2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="E2">
+        <v>50</v>
+      </c>
+      <c r="F2">
+        <v>30</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>100</v>
@@ -968,25 +999,31 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B6">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -995,15 +1032,95 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B8">
         <v>100</v>
       </c>
       <c r="C8">
         <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>35</v>
+      </c>
+      <c r="E9">
+        <v>45</v>
+      </c>
+      <c r="F9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10">
+        <v>100</v>
+      </c>
+      <c r="C10">
+        <v>90</v>
+      </c>
+      <c r="D10">
+        <v>70</v>
+      </c>
+      <c r="E10">
+        <v>50</v>
+      </c>
+      <c r="F10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>100</v>
+      </c>
+      <c r="C12">
+        <v>100</v>
+      </c>
+      <c r="D12">
+        <v>100</v>
+      </c>
+      <c r="E12">
+        <v>100</v>
+      </c>
+      <c r="F12">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1015,47 +1132,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF1C241F-6D3F-42E9-8DF6-C80C18453197}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>27</v>
-      </c>
-      <c r="D1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B2">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="C2">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D2">
         <v>100</v>
@@ -1067,29 +1184,29 @@
         <v>100</v>
       </c>
       <c r="G2">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="H2">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>100</v>
@@ -1110,8 +1227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{630D2237-30A6-4886-A54B-80E34ED32BA8}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1121,19 +1238,19 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1">
+        <v>15</v>
+      </c>
+      <c r="D1">
         <v>20</v>
       </c>
-      <c r="D1">
-        <v>30</v>
-      </c>
       <c r="E1">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="F1">
         <v>100</v>
@@ -1141,7 +1258,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -1161,19 +1278,19 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F3">
         <v>12</v>
@@ -1184,7 +1301,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <v>100</v>
@@ -1207,21 +1324,21 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <v>100</v>
@@ -1242,35 +1359,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1360E969-6246-4B45-A0C1-A28BCA2343CA}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C1">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D1">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E1">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="F1">
-        <v>100</v>
+        <v>500</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -1290,19 +1407,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B3">
+        <v>0.1</v>
+      </c>
+      <c r="C3">
+        <v>0.2</v>
+      </c>
+      <c r="D3">
         <v>1</v>
       </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>10</v>
-      </c>
       <c r="E3">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="F3">
         <v>100</v>
@@ -1310,7 +1427,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B4">
         <v>100</v>
@@ -1330,21 +1447,21 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <v>100</v>
@@ -1363,87 +1480,124 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE727A56-6128-40D3-B114-446A30773FF7}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B1">
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="C1">
+        <v>85</v>
+      </c>
+      <c r="D1">
         <v>70</v>
       </c>
-      <c r="D1">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1">
+        <v>30</v>
+      </c>
+      <c r="F1">
+        <v>20</v>
+      </c>
+      <c r="G1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B2">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C2">
         <v>90</v>
       </c>
       <c r="D2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="E2">
+        <v>50</v>
+      </c>
+      <c r="F2">
+        <v>30</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>35</v>
+      </c>
+      <c r="E3">
+        <v>45</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4">
+        <v>100</v>
+      </c>
+      <c r="C4">
+        <v>90</v>
+      </c>
+      <c r="D4">
+        <v>70</v>
+      </c>
+      <c r="E4">
+        <v>50</v>
+      </c>
+      <c r="F4">
         <v>10</v>
       </c>
-      <c r="C3">
-        <v>30</v>
-      </c>
-      <c r="D3">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4">
-        <v>100</v>
-      </c>
-      <c r="C4">
-        <v>35</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <v>100</v>
@@ -1455,37 +1609,49 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>0</v>
       </c>
-      <c r="C7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
       <c r="B8">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="C8">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="D8">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="F8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1494,9 +1660,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B10">
         <v>100</v>
@@ -1508,4 +1674,283 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008864D41C708CC54AABC64DB9F8EC5160" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8280e7c680d5d724f4413038ca100d1d">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="aecedfd1-a701-4d39-be9b-da32a8dfc2a5" xmlns:ns3="6cc8ca2e-56d8-406d-8e41-68c6b727753a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a78283ead66d0e44d8e1b525c3947135" ns2:_="" ns3:_="">
+    <xsd:import namespace="aecedfd1-a701-4d39-be9b-da32a8dfc2a5"/>
+    <xsd:import namespace="6cc8ca2e-56d8-406d-8e41-68c6b727753a"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="aecedfd1-a701-4d39-be9b-da32a8dfc2a5" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="15" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="f70eea2c-645a-430f-a841-8bf9f54459d2" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="17" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="18" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="19" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="20" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="21" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="22" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="23" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="6cc8ca2e-56d8-406d-8e41-68c6b727753a" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="12" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="13" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="16" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{c652e84b-2902-41ff-b436-4ac31d16ee34}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="6cc8ca2e-56d8-406d-8e41-68c6b727753a">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E90797E5-942B-46E7-AC7C-98401B9FAE02}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="aecedfd1-a701-4d39-be9b-da32a8dfc2a5"/>
+    <ds:schemaRef ds:uri="6cc8ca2e-56d8-406d-8e41-68c6b727753a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C46AB070-37E3-482F-BB4D-3362F6C5151B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>